<commit_message>
changed for new assignment needs
</commit_message>
<xml_diff>
--- a/eoq_results.xlsx
+++ b/eoq_results.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="39">
   <si>
     <t>Parameter</t>
   </si>
@@ -23,7 +23,7 @@
     <t>Value</t>
   </si>
   <si>
-    <t>Demand Rate (units/week)</t>
+    <t>Demand Rate (units/day)</t>
   </si>
   <si>
     <t>Demand Yearly (units/year)</t>
@@ -35,13 +35,19 @@
     <t>Holding Cost Rate (annual %)</t>
   </si>
   <si>
+    <t>Holding Cost per Unit (dollars/unit/year)</t>
+  </si>
+  <si>
     <t>Ordering Cost (dollars/order)</t>
   </si>
   <si>
     <t>Standard Deviation (units/week)</t>
   </si>
   <si>
-    <t>Lead Time (weeks)</t>
+    <t>Standard Deviation (units/day)</t>
+  </si>
+  <si>
+    <t>Lead Time (days)</t>
   </si>
   <si>
     <t>Service Level (%)</t>
@@ -50,9 +56,18 @@
     <t>Weeks per Year</t>
   </si>
   <si>
+    <t>Days per Year</t>
+  </si>
+  <si>
     <t>EOQ</t>
   </si>
   <si>
+    <t>Toggle Holding Stock</t>
+  </si>
+  <si>
+    <t>Z Score</t>
+  </si>
+  <si>
     <t>Calculation</t>
   </si>
   <si>
@@ -74,31 +89,37 @@
     <t>Safety Stock (units)</t>
   </si>
   <si>
-    <t>Time Between Orders (weeks)</t>
+    <t>Time Between Orders (days)</t>
   </si>
   <si>
     <t>Reorder Point (ROP)</t>
   </si>
   <si>
+    <t>Number of Orders per Year</t>
+  </si>
+  <si>
     <t>Given</t>
   </si>
   <si>
-    <t>Demand Rate * Weeks per Year</t>
-  </si>
-  <si>
-    <t>sqrt((2 * Demand Yearly * Ordering Cost) / Annual Holding Cost)</t>
-  </si>
-  <si>
-    <t>(EOQ / 2) * Annual Holding Cost</t>
+    <t>Demand Rate * Days per Year</t>
+  </si>
+  <si>
+    <t>Holding Cost Rate * Purchase Cost</t>
+  </si>
+  <si>
+    <t>sqrt((2 * Demand Yearly * Ordering Cost) / (Holding Cost per Unit))</t>
+  </si>
+  <si>
+    <t>(EOQ / 2) * Holding Cost per Unit</t>
   </si>
   <si>
     <t>(Demand Yearly / EOQ) * Ordering Cost</t>
   </si>
   <si>
-    <t>Safety Stock * Annual Holding Cost</t>
-  </si>
-  <si>
-    <t>Annual Holding Cost + Annual Ordering Cost + Annual Safety Stock Cost</t>
+    <t>Safety Stock * Holding Cost per Unit</t>
+  </si>
+  <si>
+    <t>Annual Holding Cost + Annual Ordering Cost + (Annual Safety Stock Cost if applicable)</t>
   </si>
   <si>
     <t>z * sigma_dLT</t>
@@ -108,12 +129,18 @@
   </si>
   <si>
     <t>Demand Rate * Lead Time + Safety Stock</t>
+  </si>
+  <si>
+    <t>Demand Yearly / EOQ</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.00"/>
+  </numFmts>
   <fonts count="2">
     <font>
       <sz val="11"/>
@@ -166,11 +193,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -210,7 +238,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1828800" y="190500"/>
+          <a:off x="6810375" y="190500"/>
           <a:ext cx="9144018" cy="5486411"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -508,11 +536,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="30.7109375" customWidth="1"/>
+    <col min="2" max="2" width="20.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
@@ -527,7 +559,7 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -540,7 +572,7 @@
         <v>4</v>
       </c>
       <c r="B4">
-        <v>60</v>
+        <v>11.7</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -548,39 +580,33 @@
         <v>5</v>
       </c>
       <c r="B5">
-        <v>0.25</v>
+        <v>0.28</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
         <v>6</v>
       </c>
-      <c r="B6">
-        <v>45</v>
-      </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
         <v>7</v>
       </c>
       <c r="B7">
-        <v>5</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
         <v>8</v>
       </c>
-      <c r="B8">
-        <v>2</v>
-      </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
         <v>9</v>
       </c>
       <c r="B9">
-        <v>90</v>
+        <v>6.124</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -588,7 +614,7 @@
         <v>10</v>
       </c>
       <c r="B10">
-        <v>52</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -596,7 +622,47 @@
         <v>11</v>
       </c>
       <c r="B11">
-        <v>74.93997598078077</v>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12">
+        <v>44.57142857142857</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14">
+        <v>392.7922024247862</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16">
+        <v>0.8416212335729143</v>
       </c>
     </row>
   </sheetData>
@@ -606,11 +672,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="40.7109375" customWidth="1"/>
+    <col min="2" max="2" width="20.7109375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="40.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
@@ -620,161 +691,188 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2">
-        <v>18</v>
+      <c r="B2" s="2">
+        <v>15</v>
       </c>
       <c r="C2" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
-      <c r="B3">
-        <v>936</v>
-      </c>
       <c r="C3" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
         <v>4</v>
       </c>
-      <c r="B4">
-        <v>60</v>
+      <c r="B4" s="2">
+        <v>11.7</v>
       </c>
       <c r="C4" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
         <v>5</v>
       </c>
-      <c r="B5">
-        <v>0.25</v>
+      <c r="B5" s="2">
+        <v>0.28</v>
       </c>
       <c r="C5" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
         <v>6</v>
       </c>
-      <c r="B6">
-        <v>45</v>
-      </c>
       <c r="C6" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7">
-        <v>52</v>
+        <v>7</v>
+      </c>
+      <c r="B7" s="2">
+        <v>54</v>
       </c>
       <c r="C7" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8">
-        <v>74.93997598078077</v>
+        <v>12</v>
+      </c>
+      <c r="B8" s="2">
+        <v>44.57142857142857</v>
       </c>
       <c r="C8" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>14</v>
-      </c>
-      <c r="B9">
-        <v>562</v>
+        <v>13</v>
+      </c>
+      <c r="B9" s="2">
+        <v>312</v>
       </c>
       <c r="C9" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>15</v>
-      </c>
-      <c r="B10">
-        <v>562</v>
+        <v>18</v>
+      </c>
+      <c r="B10" s="2">
+        <v>392.7922024247862</v>
       </c>
       <c r="C10" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>16</v>
-      </c>
-      <c r="B11">
-        <v>135</v>
+        <v>19</v>
+      </c>
+      <c r="B11" s="2">
+        <v>643.4</v>
       </c>
       <c r="C11" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" t="s">
-        <v>17</v>
-      </c>
-      <c r="B12">
-        <v>1259</v>
+        <v>20</v>
+      </c>
+      <c r="B12" s="2">
+        <v>643.4</v>
       </c>
       <c r="C12" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" t="s">
-        <v>18</v>
-      </c>
-      <c r="B13">
-        <v>9</v>
+        <v>21</v>
+      </c>
+      <c r="B13" s="2">
+        <v>27.2</v>
       </c>
       <c r="C13" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" t="s">
-        <v>19</v>
-      </c>
-      <c r="B14">
-        <v>4</v>
+        <v>22</v>
+      </c>
+      <c r="B14" s="2">
+        <v>1314</v>
       </c>
       <c r="C14" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" t="s">
-        <v>20</v>
-      </c>
-      <c r="B15">
-        <v>45</v>
+        <v>23</v>
+      </c>
+      <c r="B15" s="2">
+        <v>8.300000000000001</v>
       </c>
       <c r="C15" t="s">
-        <v>30</v>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" t="s">
+        <v>24</v>
+      </c>
+      <c r="B16" s="2">
+        <v>26.2</v>
+      </c>
+      <c r="C16" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" t="s">
+        <v>25</v>
+      </c>
+      <c r="B17" s="2">
+        <v>278.3</v>
+      </c>
+      <c r="C17" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" t="s">
+        <v>26</v>
+      </c>
+      <c r="B18" s="2">
+        <v>11.9</v>
+      </c>
+      <c r="C18" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>